<commit_message>
Added specs for table
</commit_message>
<xml_diff>
--- a/test/integrated/demo.xlsx
+++ b/test/integrated/demo.xlsx
@@ -1,9 +1,3 @@
-
-<file path=workbook/sheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetData/>
-</worksheet>
-</file>
 
 <file path=workbook/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">

</xml_diff>

<commit_message>
Add fillSpec and numFormatSpec
</commit_message>
<xml_diff>
--- a/test/integrated/demo.xlsx
+++ b/test/integrated/demo.xlsx
@@ -1,3 +1,9 @@
+
+<file path=workbook/sheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetData/>
+</worksheet>
+</file>
 
 <file path=workbook/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">

</xml_diff>